<commit_message>
Change Structre + Test
</commit_message>
<xml_diff>
--- a/TruckList.xlsx
+++ b/TruckList.xlsx
@@ -1,37 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dormandode-my.sharepoint.com/personal/tom_konieczny_emma-sleep_com/Documents/Dokumente/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D82F71A6-C9CD-41BB-99F3-3EFD547F74F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" xr2:uid="{909D980A-458C-4EC0-842B-D6EA8477C21F}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -98,42 +76,50 @@
     <t>x</t>
   </si>
   <si>
+    <t>EMAHE080200AAA</t>
+  </si>
+  <si>
+    <t>EMAHE090200AAA</t>
+  </si>
+  <si>
+    <t>EMAHE090210AAA</t>
+  </si>
+  <si>
+    <t>EMAHE140200AAA</t>
+  </si>
+  <si>
+    <t>EMAHE160200AAA</t>
+  </si>
+  <si>
+    <t>EMAHE180200AAA</t>
+  </si>
+  <si>
     <t>Uden</t>
   </si>
   <si>
     <t>12.07.2024</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>EMAHE080200AAA</t>
-  </si>
-  <si>
-    <t>EMAHE090200AAA</t>
-  </si>
-  <si>
-    <t>EMAHE090210AAA</t>
-  </si>
-  <si>
-    <t>EMAHE140200AAA</t>
-  </si>
-  <si>
-    <t>EMAHE160200AAA</t>
-  </si>
-  <si>
-    <t>EMAHE180200AAA</t>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -146,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -154,26 +140,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -188,44 +184,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -252,32 +248,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -304,24 +282,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -333,226 +293,228 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr"/>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EEBA469-5CCA-4FFC-B906-B6797F027D45}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -572,7 +534,7 @@
         <v>1197041</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <v>42</v>
@@ -581,16 +543,16 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="P2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -610,7 +572,7 @@
         <v>1197040</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H3">
         <v>102</v>
@@ -619,16 +581,16 @@
         <v>2</v>
       </c>
       <c r="N3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="P3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -648,7 +610,7 @@
         <v>1197038</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H4">
         <v>60</v>
@@ -657,16 +619,16 @@
         <v>3</v>
       </c>
       <c r="N4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="P4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -686,7 +648,7 @@
         <v>1197044</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H5">
         <v>114</v>
@@ -695,16 +657,16 @@
         <v>4</v>
       </c>
       <c r="N5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="P5" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -724,7 +686,7 @@
         <v>1197039</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H6">
         <v>102</v>
@@ -733,16 +695,16 @@
         <v>5</v>
       </c>
       <c r="N6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="P6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -762,7 +724,7 @@
         <v>1197032</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H7">
         <v>96</v>
@@ -771,13 +733,13 @@
         <v>6</v>
       </c>
       <c r="N7" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="P7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>